<commit_message>
"Cucumber Class 8 screenshots"
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch12excel.xlsx
+++ b/src/test/resources/testdata/batch12excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quytr\IdeaProjects\CucumberFrameworkBatch12\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65CC522-53C2-44A1-89CA-706B49E3F7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A8809-C0E1-41EB-80C2-9818661D0F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1935" windowWidth="18960" windowHeight="13020" xr2:uid="{6F8F12F9-0F58-41A1-B0C5-C42D0B39478B}"/>
   </bookViews>
@@ -70,25 +70,25 @@
     <t>C:\Users\quytr\Desktop\Batch12\imagebatch12.jpg</t>
   </si>
   <si>
-    <t>Adel</t>
-  </si>
-  <si>
-    <t>Croir</t>
-  </si>
-  <si>
-    <t>Hufae</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
-    <t>crisms123</t>
-  </si>
-  <si>
-    <t>kra321</t>
-  </si>
-  <si>
-    <t>sudn987</t>
+    <t>Adeyy</t>
+  </si>
+  <si>
+    <t>Poef</t>
+  </si>
+  <si>
+    <t>Lofd</t>
+  </si>
+  <si>
+    <t>crewr354</t>
+  </si>
+  <si>
+    <t>ftry3</t>
+  </si>
+  <si>
+    <t>suhn35</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>

</xml_diff>